<commit_message>
read volume and number of parts in the same file not in CP
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/volumeOARs/OAR-man.xlsx
+++ b/Plancheck/plancheck_data/volumeOARs/OAR-man.xlsx
@@ -26,97 +26,97 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
-    <t>Coeur(vol)</t>
-  </si>
-  <si>
-    <t>Poumons(vol)</t>
-  </si>
-  <si>
-    <t>PoumonDt(vol)</t>
-  </si>
-  <si>
-    <t>PoumonGche(vol)</t>
-  </si>
-  <si>
-    <t>Vessie(vol)</t>
-  </si>
-  <si>
-    <t>Rectum(vol)</t>
-  </si>
-  <si>
-    <t>Grele(vol)</t>
-  </si>
-  <si>
-    <t>Sigmoide(vol)</t>
-  </si>
-  <si>
-    <t>Oesophage(vol)</t>
-  </si>
-  <si>
-    <t>Foie(vol)</t>
-  </si>
-  <si>
-    <t>Chiasma(vol)</t>
-  </si>
-  <si>
-    <t>NerfOptiqueGche(vol)</t>
-  </si>
-  <si>
-    <t>NerfOptiqueDt(vol)</t>
-  </si>
-  <si>
-    <t>Cerveau(vol)</t>
-  </si>
-  <si>
-    <t>CristallinDt(vol)</t>
-  </si>
-  <si>
-    <t>CristallinGche(vol)</t>
-  </si>
-  <si>
-    <t>OeilDt(vol)</t>
-  </si>
-  <si>
-    <t>OeilGche(vol)</t>
-  </si>
-  <si>
-    <t>Canal Med(vol)</t>
-  </si>
-  <si>
-    <t>Cav Buc(vol)</t>
-  </si>
-  <si>
-    <t>ParoDte(vol)</t>
-  </si>
-  <si>
-    <t>ParoGche(vol)</t>
-  </si>
-  <si>
-    <t>PlexusDt(vol)</t>
-  </si>
-  <si>
-    <t>PlexusGche(vol)</t>
-  </si>
-  <si>
-    <t>Estomac(vol)</t>
-  </si>
-  <si>
-    <t>ReinDt(vol)</t>
-  </si>
-  <si>
-    <t>ReinGche(vol)</t>
-  </si>
-  <si>
-    <t>TeteFemorDte(vol)</t>
-  </si>
-  <si>
-    <t>TeteFemorGche(vol)</t>
-  </si>
-  <si>
-    <t>ATMDte(vol)</t>
-  </si>
-  <si>
-    <t>ATMGche(vol)</t>
+    <t>Coeur</t>
+  </si>
+  <si>
+    <t>Poumons</t>
+  </si>
+  <si>
+    <t>PoumonDt</t>
+  </si>
+  <si>
+    <t>PoumonGche</t>
+  </si>
+  <si>
+    <t>Vessie</t>
+  </si>
+  <si>
+    <t>Rectum</t>
+  </si>
+  <si>
+    <t>Grele</t>
+  </si>
+  <si>
+    <t>Sigmoide</t>
+  </si>
+  <si>
+    <t>Oesophage</t>
+  </si>
+  <si>
+    <t>Foie</t>
+  </si>
+  <si>
+    <t>Chiasma</t>
+  </si>
+  <si>
+    <t>NerfOptiqueGche</t>
+  </si>
+  <si>
+    <t>NerfOptiqueDt</t>
+  </si>
+  <si>
+    <t>Cerveau</t>
+  </si>
+  <si>
+    <t>CristallinDt</t>
+  </si>
+  <si>
+    <t>CristallinGche</t>
+  </si>
+  <si>
+    <t>OeilDt</t>
+  </si>
+  <si>
+    <t>OeilGche</t>
+  </si>
+  <si>
+    <t>Canal Med</t>
+  </si>
+  <si>
+    <t>Cav Buc</t>
+  </si>
+  <si>
+    <t>ParoDte</t>
+  </si>
+  <si>
+    <t>ParoGche</t>
+  </si>
+  <si>
+    <t>PlexusDt</t>
+  </si>
+  <si>
+    <t>PlexusGche</t>
+  </si>
+  <si>
+    <t>Estomac</t>
+  </si>
+  <si>
+    <t>ReinDt</t>
+  </si>
+  <si>
+    <t>ReinGche</t>
+  </si>
+  <si>
+    <t>TeteFemorDte</t>
+  </si>
+  <si>
+    <t>TeteFemorGche</t>
+  </si>
+  <si>
+    <t>ATMDte</t>
+  </si>
+  <si>
+    <t>ATMGche</t>
   </si>
 </sst>
 </file>

</xml_diff>